<commit_message>
Update Work Log 2023-24A ADS_AI(1).xlsx
</commit_message>
<xml_diff>
--- a/Deliverables/Work Log 2023-24A ADS_AI(1).xlsx
+++ b/Deliverables/Work Log 2023-24A ADS_AI(1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larsk\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larsk\GitHub\LarsKerkhofs_GitHubExercise\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C29BEF-FB4D-4537-9E2F-26C8CA6A1FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE3A00A-7729-4BD2-A2CF-C70B37A723E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="184">
   <si>
     <t>Date</t>
   </si>
@@ -1071,17 +1071,37 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1095,34 +1115,14 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1580,8 +1580,8 @@
   <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B145" sqref="B145"/>
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J147" sqref="J147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1634,7 +1634,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="69" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="52"/>
@@ -1652,35 +1652,35 @@
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="55"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
     </row>
     <row r="4" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="57"/>
     </row>
     <row r="5" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A5" s="33">
@@ -2027,7 +2027,7 @@
       <c r="K15" s="21"/>
     </row>
     <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="56" t="s">
+      <c r="A16" s="71" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="52"/>
@@ -2045,35 +2045,35 @@
       <c r="A17" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="55"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="57"/>
     </row>
     <row r="18" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="55"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="57"/>
     </row>
     <row r="19" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
@@ -2392,53 +2392,53 @@
       <c r="K29" s="21"/>
     </row>
     <row r="30" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="58" t="s">
+      <c r="A30" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="55"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="57"/>
     </row>
     <row r="31" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="59" t="s">
+      <c r="B31" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="55"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="57"/>
     </row>
     <row r="32" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="59" t="s">
+      <c r="B32" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="54"/>
-      <c r="I32" s="54"/>
-      <c r="J32" s="54"/>
-      <c r="K32" s="55"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="56"/>
+      <c r="K32" s="57"/>
     </row>
     <row r="33" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A33" s="33">
@@ -2854,53 +2854,53 @@
       <c r="K45" s="21"/>
     </row>
     <row r="46" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="60" t="s">
+      <c r="A46" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="B46" s="54"/>
-      <c r="C46" s="54"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="54"/>
-      <c r="F46" s="54"/>
-      <c r="G46" s="54"/>
-      <c r="H46" s="54"/>
-      <c r="I46" s="54"/>
-      <c r="J46" s="54"/>
-      <c r="K46" s="55"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="56"/>
+      <c r="G46" s="56"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
+      <c r="K46" s="57"/>
     </row>
     <row r="47" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="61" t="s">
+      <c r="B47" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="C47" s="54"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="54"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="54"/>
-      <c r="H47" s="54"/>
-      <c r="I47" s="54"/>
-      <c r="J47" s="54"/>
-      <c r="K47" s="55"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="56"/>
+      <c r="G47" s="56"/>
+      <c r="H47" s="56"/>
+      <c r="I47" s="56"/>
+      <c r="J47" s="56"/>
+      <c r="K47" s="57"/>
     </row>
     <row r="48" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="61" t="s">
+      <c r="B48" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="54"/>
-      <c r="D48" s="54"/>
-      <c r="E48" s="54"/>
-      <c r="F48" s="54"/>
-      <c r="G48" s="54"/>
-      <c r="H48" s="54"/>
-      <c r="I48" s="54"/>
-      <c r="J48" s="54"/>
-      <c r="K48" s="55"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56"/>
+      <c r="F48" s="56"/>
+      <c r="G48" s="56"/>
+      <c r="H48" s="56"/>
+      <c r="I48" s="56"/>
+      <c r="J48" s="56"/>
+      <c r="K48" s="57"/>
     </row>
     <row r="49" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A49" s="33">
@@ -3419,53 +3419,53 @@
       <c r="K64" s="21"/>
     </row>
     <row r="65" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="62" t="s">
+      <c r="A65" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="B65" s="54"/>
-      <c r="C65" s="54"/>
-      <c r="D65" s="54"/>
-      <c r="E65" s="54"/>
-      <c r="F65" s="54"/>
-      <c r="G65" s="54"/>
-      <c r="H65" s="54"/>
-      <c r="I65" s="54"/>
-      <c r="J65" s="54"/>
-      <c r="K65" s="55"/>
+      <c r="B65" s="56"/>
+      <c r="C65" s="56"/>
+      <c r="D65" s="56"/>
+      <c r="E65" s="56"/>
+      <c r="F65" s="56"/>
+      <c r="G65" s="56"/>
+      <c r="H65" s="56"/>
+      <c r="I65" s="56"/>
+      <c r="J65" s="56"/>
+      <c r="K65" s="57"/>
     </row>
     <row r="66" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A66" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B66" s="63" t="s">
+      <c r="B66" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="C66" s="54"/>
-      <c r="D66" s="54"/>
-      <c r="E66" s="54"/>
-      <c r="F66" s="54"/>
-      <c r="G66" s="54"/>
-      <c r="H66" s="54"/>
-      <c r="I66" s="54"/>
-      <c r="J66" s="54"/>
-      <c r="K66" s="55"/>
+      <c r="C66" s="56"/>
+      <c r="D66" s="56"/>
+      <c r="E66" s="56"/>
+      <c r="F66" s="56"/>
+      <c r="G66" s="56"/>
+      <c r="H66" s="56"/>
+      <c r="I66" s="56"/>
+      <c r="J66" s="56"/>
+      <c r="K66" s="57"/>
     </row>
     <row r="67" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B67" s="63" t="s">
+      <c r="B67" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="C67" s="54"/>
-      <c r="D67" s="54"/>
-      <c r="E67" s="54"/>
-      <c r="F67" s="54"/>
-      <c r="G67" s="54"/>
-      <c r="H67" s="54"/>
-      <c r="I67" s="54"/>
-      <c r="J67" s="54"/>
-      <c r="K67" s="55"/>
+      <c r="C67" s="56"/>
+      <c r="D67" s="56"/>
+      <c r="E67" s="56"/>
+      <c r="F67" s="56"/>
+      <c r="G67" s="56"/>
+      <c r="H67" s="56"/>
+      <c r="I67" s="56"/>
+      <c r="J67" s="56"/>
+      <c r="K67" s="57"/>
     </row>
     <row r="68" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A68" s="33">
@@ -4110,53 +4110,53 @@
       <c r="K87" s="21"/>
     </row>
     <row r="88" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="68" t="s">
+      <c r="A88" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="B88" s="54"/>
-      <c r="C88" s="54"/>
-      <c r="D88" s="54"/>
-      <c r="E88" s="54"/>
-      <c r="F88" s="54"/>
-      <c r="G88" s="54"/>
-      <c r="H88" s="54"/>
-      <c r="I88" s="54"/>
-      <c r="J88" s="54"/>
-      <c r="K88" s="55"/>
+      <c r="B88" s="56"/>
+      <c r="C88" s="56"/>
+      <c r="D88" s="56"/>
+      <c r="E88" s="56"/>
+      <c r="F88" s="56"/>
+      <c r="G88" s="56"/>
+      <c r="H88" s="56"/>
+      <c r="I88" s="56"/>
+      <c r="J88" s="56"/>
+      <c r="K88" s="57"/>
     </row>
     <row r="89" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A89" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B89" s="69" t="s">
+      <c r="B89" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="C89" s="54"/>
-      <c r="D89" s="54"/>
-      <c r="E89" s="54"/>
-      <c r="F89" s="54"/>
-      <c r="G89" s="54"/>
-      <c r="H89" s="54"/>
-      <c r="I89" s="54"/>
-      <c r="J89" s="54"/>
-      <c r="K89" s="55"/>
+      <c r="C89" s="56"/>
+      <c r="D89" s="56"/>
+      <c r="E89" s="56"/>
+      <c r="F89" s="56"/>
+      <c r="G89" s="56"/>
+      <c r="H89" s="56"/>
+      <c r="I89" s="56"/>
+      <c r="J89" s="56"/>
+      <c r="K89" s="57"/>
     </row>
     <row r="90" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B90" s="69" t="s">
+      <c r="B90" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C90" s="54"/>
-      <c r="D90" s="54"/>
-      <c r="E90" s="54"/>
-      <c r="F90" s="54"/>
-      <c r="G90" s="54"/>
-      <c r="H90" s="54"/>
-      <c r="I90" s="54"/>
-      <c r="J90" s="54"/>
-      <c r="K90" s="55"/>
+      <c r="C90" s="56"/>
+      <c r="D90" s="56"/>
+      <c r="E90" s="56"/>
+      <c r="F90" s="56"/>
+      <c r="G90" s="56"/>
+      <c r="H90" s="56"/>
+      <c r="I90" s="56"/>
+      <c r="J90" s="56"/>
+      <c r="K90" s="57"/>
     </row>
     <row r="91" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A91" s="33">
@@ -4756,53 +4756,53 @@
       <c r="K109" s="21"/>
     </row>
     <row r="110" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="70" t="s">
+      <c r="A110" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="B110" s="54"/>
-      <c r="C110" s="54"/>
-      <c r="D110" s="54"/>
-      <c r="E110" s="54"/>
-      <c r="F110" s="54"/>
-      <c r="G110" s="54"/>
-      <c r="H110" s="54"/>
-      <c r="I110" s="54"/>
-      <c r="J110" s="54"/>
-      <c r="K110" s="55"/>
+      <c r="B110" s="56"/>
+      <c r="C110" s="56"/>
+      <c r="D110" s="56"/>
+      <c r="E110" s="56"/>
+      <c r="F110" s="56"/>
+      <c r="G110" s="56"/>
+      <c r="H110" s="56"/>
+      <c r="I110" s="56"/>
+      <c r="J110" s="56"/>
+      <c r="K110" s="57"/>
     </row>
     <row r="111" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A111" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B111" s="71" t="s">
+      <c r="B111" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="C111" s="54"/>
-      <c r="D111" s="54"/>
-      <c r="E111" s="54"/>
-      <c r="F111" s="54"/>
-      <c r="G111" s="54"/>
-      <c r="H111" s="54"/>
-      <c r="I111" s="54"/>
-      <c r="J111" s="54"/>
-      <c r="K111" s="55"/>
+      <c r="C111" s="56"/>
+      <c r="D111" s="56"/>
+      <c r="E111" s="56"/>
+      <c r="F111" s="56"/>
+      <c r="G111" s="56"/>
+      <c r="H111" s="56"/>
+      <c r="I111" s="56"/>
+      <c r="J111" s="56"/>
+      <c r="K111" s="57"/>
     </row>
     <row r="112" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B112" s="71" t="s">
+      <c r="B112" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="C112" s="54"/>
-      <c r="D112" s="54"/>
-      <c r="E112" s="54"/>
-      <c r="F112" s="54"/>
-      <c r="G112" s="54"/>
-      <c r="H112" s="54"/>
-      <c r="I112" s="54"/>
-      <c r="J112" s="54"/>
-      <c r="K112" s="55"/>
+      <c r="C112" s="56"/>
+      <c r="D112" s="56"/>
+      <c r="E112" s="56"/>
+      <c r="F112" s="56"/>
+      <c r="G112" s="56"/>
+      <c r="H112" s="56"/>
+      <c r="I112" s="56"/>
+      <c r="J112" s="56"/>
+      <c r="K112" s="57"/>
     </row>
     <row r="113" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A113" s="33">
@@ -5338,22 +5338,22 @@
       <c r="A130" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="B130" s="54"/>
-      <c r="C130" s="54"/>
-      <c r="D130" s="54"/>
-      <c r="E130" s="54"/>
-      <c r="F130" s="54"/>
-      <c r="G130" s="54"/>
-      <c r="H130" s="54"/>
-      <c r="I130" s="54"/>
-      <c r="J130" s="54"/>
-      <c r="K130" s="55"/>
+      <c r="B130" s="56"/>
+      <c r="C130" s="56"/>
+      <c r="D130" s="56"/>
+      <c r="E130" s="56"/>
+      <c r="F130" s="56"/>
+      <c r="G130" s="56"/>
+      <c r="H130" s="56"/>
+      <c r="I130" s="56"/>
+      <c r="J130" s="56"/>
+      <c r="K130" s="57"/>
     </row>
     <row r="131" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A131" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B131" s="65" t="s">
+      <c r="B131" s="51" t="s">
         <v>13</v>
       </c>
       <c r="C131" s="52"/>
@@ -5364,13 +5364,13 @@
       <c r="H131" s="52"/>
       <c r="I131" s="52"/>
       <c r="J131" s="52"/>
-      <c r="K131" s="66"/>
+      <c r="K131" s="53"/>
     </row>
     <row r="132" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="B132" s="67" t="s">
+      <c r="B132" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C132" s="52"/>
@@ -5381,7 +5381,7 @@
       <c r="H132" s="52"/>
       <c r="I132" s="52"/>
       <c r="J132" s="52"/>
-      <c r="K132" s="66"/>
+      <c r="K132" s="53"/>
     </row>
     <row r="133" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A133" s="33">
@@ -5802,16 +5802,30 @@
       <c r="K145" s="28"/>
     </row>
     <row r="146" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A146" s="33"/>
-      <c r="B146" s="28"/>
+      <c r="A146" s="33">
+        <v>45232</v>
+      </c>
+      <c r="B146" s="28" t="s">
+        <v>50</v>
+      </c>
       <c r="C146" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D146" s="28"/>
-      <c r="E146" s="13"/>
-      <c r="F146" s="13"/>
-      <c r="G146" s="30"/>
-      <c r="H146" s="30"/>
+      <c r="D146" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="E146" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F146" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G146" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="H146" s="30">
+        <v>0.5</v>
+      </c>
       <c r="I146" s="30">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -5866,11 +5880,11 @@
       <c r="F149" s="21"/>
       <c r="G149" s="24">
         <f t="shared" ref="G149:H149" si="9">SUM(G133:G148)</f>
-        <v>29.5</v>
+        <v>30</v>
       </c>
       <c r="H149" s="24">
         <f t="shared" si="9"/>
-        <v>29.5</v>
+        <v>30</v>
       </c>
       <c r="I149" s="24">
         <f t="shared" si="8"/>
@@ -5891,11 +5905,11 @@
       <c r="F151" s="45"/>
       <c r="G151" s="46">
         <f>G15+G29+G45+G64+G87+G109+G129+G149</f>
-        <v>154.80000000000001</v>
+        <v>155.30000000000001</v>
       </c>
       <c r="H151" s="46">
         <f>H15+H29+H45+H64+H87+H109+H129+H149</f>
-        <v>170.3</v>
+        <v>170.8</v>
       </c>
       <c r="I151" s="46">
         <f>H151-G151</f>
@@ -5907,7 +5921,7 @@
   <customSheetViews>
     <customSheetView guid="{8BAC9A6B-5D32-4E8D-967D-E17D357516F8}" filter="1" showAutoFilter="1">
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="A1:K15" xr:uid="{2FCD0418-5B78-4308-A256-C801BCFEF926}">
+      <autoFilter ref="A1:K15" xr:uid="{507131DC-EED8-4FA3-9AFB-FE4DA244CFE5}">
         <filterColumn colId="1">
           <filters blank="1">
             <filter val="- Weekplan item 1_x000a_- Weekplan item 2_x000a_- Weekplan item 3_x000a_- etc"/>
@@ -5918,6 +5932,21 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="24">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="A16:K16"/>
+    <mergeCell ref="B17:K17"/>
+    <mergeCell ref="B18:K18"/>
+    <mergeCell ref="A30:K30"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="B32:K32"/>
+    <mergeCell ref="A46:K46"/>
+    <mergeCell ref="B47:K47"/>
+    <mergeCell ref="B48:K48"/>
+    <mergeCell ref="A65:K65"/>
+    <mergeCell ref="B66:K66"/>
+    <mergeCell ref="A130:K130"/>
     <mergeCell ref="B131:K131"/>
     <mergeCell ref="B132:K132"/>
     <mergeCell ref="B67:K67"/>
@@ -5927,21 +5956,6 @@
     <mergeCell ref="A110:K110"/>
     <mergeCell ref="B111:K111"/>
     <mergeCell ref="B112:K112"/>
-    <mergeCell ref="B47:K47"/>
-    <mergeCell ref="B48:K48"/>
-    <mergeCell ref="A65:K65"/>
-    <mergeCell ref="B66:K66"/>
-    <mergeCell ref="A130:K130"/>
-    <mergeCell ref="B18:K18"/>
-    <mergeCell ref="A30:K30"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="B32:K32"/>
-    <mergeCell ref="A46:K46"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="A16:K16"/>
-    <mergeCell ref="B17:K17"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:B14 B17:B28 B33:B44 B49:B63 B68:B86 B91:B108 B113:B128 B133:B148">
     <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="Unplanned">
@@ -6018,9 +6032,10 @@
     <hyperlink ref="J92" r:id="rId13" xr:uid="{AFE1D8ED-8BDB-408D-BDFB-19B4F6566505}"/>
     <hyperlink ref="J99" r:id="rId14" xr:uid="{E09C16E1-E5CF-4AE9-895D-C3DD5D8A5980}"/>
     <hyperlink ref="J143" r:id="rId15" xr:uid="{57EB1717-BDAF-45C8-8962-0B762D06B891}"/>
+    <hyperlink ref="J62" r:id="rId16" xr:uid="{145AC5D8-792E-4CCB-BF6F-41A565AE94FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" r:id="rId16"/>
+  <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" r:id="rId17"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -7456,15 +7471,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100378F7411FF5BA04C8BB948E4423DB960" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="713ce497b2b4d71f6b5d130b802d4e8d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cafc3e4c-b146-46b8-8a52-78ced9164e87" xmlns:ns3="35914ba8-9e4a-4224-9594-5062124be8f1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b65c5356acc1011e5a91a9ea20701c21" ns2:_="" ns3:_="">
     <xsd:import namespace="cafc3e4c-b146-46b8-8a52-78ced9164e87"/>
@@ -7673,6 +7679,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7685,14 +7700,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67A64A65-7DA4-4AE1-9847-B817073E4705}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14386F84-98B0-4EBE-8663-84C7674BA9A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7711,6 +7718,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67A64A65-7DA4-4AE1-9847-B817073E4705}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{320CF63A-30C9-4A8C-8DF9-EA62B8EC1A62}">
   <ds:schemaRefs>

</xml_diff>